<commit_message>
Removing the  console for token
</commit_message>
<xml_diff>
--- a/database/Payroll-Template_2025-12-19.xlsx
+++ b/database/Payroll-Template_2025-12-19.xlsx
@@ -35,20 +35,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="13">
+  <numFmts count="1">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@"/>
-    <numFmt numFmtId="166" formatCode="mmm\ d\,\ yyyy"/>
-    <numFmt numFmtId="169" formatCode="[$₱]#,##0.00"/>
-    <numFmt numFmtId="170" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??.0_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="172" formatCode="dd\-mmm\-yy"/>
-    <numFmt numFmtId="173" formatCode="mm/dd/yyyy"/>
-    <numFmt numFmtId="174" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??.00_);_(@_)"/>
-    <numFmt numFmtId="175" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="mmmm\ d\,\ yyyy"/>
-    <numFmt numFmtId="177" formatCode="ddd\,\ mmm\ d\,\ yyyy"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -412,29 +400,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AH8"/>
+  <dimension ref="A1:CL8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="15.00390625" customWidth="1"/>
-    <col min="2" max="2" width="66.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.00390625" customWidth="1"/>
+    <col min="2" max="2" width="50.00390625" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" customWidth="1"/>
-    <col min="7" max="7" width="10.1640625" customWidth="1"/>
-    <col min="8" max="8" width="10.1640625" customWidth="1"/>
-    <col min="9" max="9" width="10.1640625" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" customWidth="1"/>
     <col min="10" max="10" width="10.1640625" customWidth="1"/>
     <col min="11" max="11" width="10.1640625" customWidth="1"/>
     <col min="12" max="12" width="10.1640625" customWidth="1"/>
-    <col min="13" max="13" width="11.33203125" customWidth="1"/>
-    <col min="14" max="14" width="11.33203125" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" customWidth="1"/>
-    <col min="16" max="16" width="11.33203125" customWidth="1"/>
-    <col min="17" max="17" width="11.33203125" customWidth="1"/>
-    <col min="18" max="18" width="11.33203125" customWidth="1"/>
+    <col min="13" max="13" width="10.1640625" customWidth="1"/>
+    <col min="14" max="14" width="10.1640625" customWidth="1"/>
+    <col min="15" max="15" width="10.1640625" customWidth="1"/>
+    <col min="16" max="16" width="10.1640625" customWidth="1"/>
+    <col min="17" max="17" width="10.1640625" customWidth="1"/>
+    <col min="18" max="18" width="10.1640625" customWidth="1"/>
     <col min="19" max="19" width="11.33203125" customWidth="1"/>
     <col min="20" max="20" width="11.33203125" customWidth="1"/>
     <col min="21" max="21" width="11.33203125" customWidth="1"/>
@@ -450,7 +438,63 @@
     <col min="31" max="31" width="11.33203125" customWidth="1"/>
     <col min="32" max="32" width="11.33203125" customWidth="1"/>
     <col min="33" max="33" width="11.33203125" customWidth="1"/>
-    <col min="34" max="34" width="16.00390625" customWidth="1"/>
+    <col min="34" max="34" width="11.33203125" customWidth="1"/>
+    <col min="35" max="35" width="11.33203125" customWidth="1"/>
+    <col min="36" max="36" width="11.33203125" customWidth="1"/>
+    <col min="37" max="37" width="11.33203125" customWidth="1"/>
+    <col min="38" max="38" width="11.33203125" customWidth="1"/>
+    <col min="39" max="39" width="11.33203125" customWidth="1"/>
+    <col min="40" max="40" width="10.1640625" customWidth="1"/>
+    <col min="41" max="41" width="10.1640625" customWidth="1"/>
+    <col min="42" max="42" width="10.1640625" customWidth="1"/>
+    <col min="43" max="43" width="10.1640625" customWidth="1"/>
+    <col min="44" max="44" width="10.1640625" customWidth="1"/>
+    <col min="45" max="45" width="10.1640625" customWidth="1"/>
+    <col min="46" max="46" width="10.1640625" customWidth="1"/>
+    <col min="47" max="47" width="10.1640625" customWidth="1"/>
+    <col min="48" max="48" width="10.1640625" customWidth="1"/>
+    <col min="49" max="49" width="11.33203125" customWidth="1"/>
+    <col min="50" max="50" width="11.33203125" customWidth="1"/>
+    <col min="51" max="51" width="11.33203125" customWidth="1"/>
+    <col min="52" max="52" width="11.33203125" customWidth="1"/>
+    <col min="53" max="53" width="11.33203125" customWidth="1"/>
+    <col min="54" max="54" width="11.33203125" customWidth="1"/>
+    <col min="55" max="55" width="11.33203125" customWidth="1"/>
+    <col min="56" max="56" width="11.33203125" customWidth="1"/>
+    <col min="57" max="57" width="11.33203125" customWidth="1"/>
+    <col min="58" max="58" width="11.33203125" customWidth="1"/>
+    <col min="59" max="59" width="11.33203125" customWidth="1"/>
+    <col min="60" max="60" width="11.33203125" customWidth="1"/>
+    <col min="61" max="61" width="11.33203125" customWidth="1"/>
+    <col min="62" max="62" width="11.33203125" customWidth="1"/>
+    <col min="63" max="63" width="11.33203125" customWidth="1"/>
+    <col min="64" max="64" width="11.33203125" customWidth="1"/>
+    <col min="65" max="65" width="11.33203125" customWidth="1"/>
+    <col min="66" max="66" width="11.33203125" customWidth="1"/>
+    <col min="67" max="67" width="11.33203125" customWidth="1"/>
+    <col min="68" max="68" width="11.33203125" customWidth="1"/>
+    <col min="69" max="69" width="11.33203125" customWidth="1"/>
+    <col min="70" max="70" width="11.33203125" customWidth="1"/>
+    <col min="71" max="71" width="10.1640625" customWidth="1"/>
+    <col min="72" max="72" width="10.1640625" customWidth="1"/>
+    <col min="73" max="73" width="10.1640625" customWidth="1"/>
+    <col min="74" max="74" width="10.1640625" customWidth="1"/>
+    <col min="75" max="75" width="10.1640625" customWidth="1"/>
+    <col min="76" max="76" width="10.1640625" customWidth="1"/>
+    <col min="77" max="77" width="10.1640625" customWidth="1"/>
+    <col min="78" max="78" width="10.1640625" customWidth="1"/>
+    <col min="79" max="79" width="10.1640625" customWidth="1"/>
+    <col min="80" max="80" width="11.33203125" customWidth="1"/>
+    <col min="81" max="81" width="11.33203125" customWidth="1"/>
+    <col min="82" max="82" width="11.33203125" customWidth="1"/>
+    <col min="83" max="83" width="11.33203125" customWidth="1"/>
+    <col min="84" max="84" width="11.33203125" customWidth="1"/>
+    <col min="85" max="85" width="11.33203125" customWidth="1"/>
+    <col min="86" max="86" width="11.33203125" customWidth="1"/>
+    <col min="87" max="87" width="11.33203125" customWidth="1"/>
+    <col min="88" max="88" width="11.33203125" customWidth="1"/>
+    <col min="89" max="89" width="11.33203125" customWidth="1"/>
+    <col min="90" max="90" width="16.00390625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="36" customHeight="1">
@@ -461,99 +505,267 @@
         <v>Employee Name</v>
       </c>
       <c r="C1" t="str">
+        <v>25-Oct-</v>
+      </c>
+      <c r="D1" t="str">
+        <v>26-Oct-</v>
+      </c>
+      <c r="E1" t="str">
+        <v>27-Oct-</v>
+      </c>
+      <c r="F1" t="str">
+        <v>28-Oct-</v>
+      </c>
+      <c r="G1" t="str">
+        <v>29-Oct-</v>
+      </c>
+      <c r="H1" t="str">
+        <v>30-Oct-</v>
+      </c>
+      <c r="I1" t="str">
+        <v>31-Oct-</v>
+      </c>
+      <c r="J1" t="str">
+        <v>1-Nov-</v>
+      </c>
+      <c r="K1" t="str">
+        <v>2-Nov-</v>
+      </c>
+      <c r="L1" t="str">
+        <v>3-Nov-</v>
+      </c>
+      <c r="M1" t="str">
+        <v>4-Nov-</v>
+      </c>
+      <c r="N1" t="str">
+        <v>5-Nov-</v>
+      </c>
+      <c r="O1" t="str">
+        <v>6-Nov-</v>
+      </c>
+      <c r="P1" t="str">
+        <v>7-Nov-</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>8-Nov-</v>
+      </c>
+      <c r="R1" t="str">
+        <v>9-Nov-</v>
+      </c>
+      <c r="S1" t="str">
+        <v>10-Nov-</v>
+      </c>
+      <c r="T1" t="str">
+        <v>11-Nov-</v>
+      </c>
+      <c r="U1" t="str">
+        <v>12-Nov-</v>
+      </c>
+      <c r="V1" t="str">
+        <v>13-Nov-</v>
+      </c>
+      <c r="W1" t="str">
+        <v>14-Nov-</v>
+      </c>
+      <c r="X1" t="str">
+        <v>15-Nov-</v>
+      </c>
+      <c r="Y1" t="str">
+        <v>16-Nov-</v>
+      </c>
+      <c r="Z1" t="str">
+        <v>17-Nov-</v>
+      </c>
+      <c r="AA1" t="str">
+        <v>18-Nov-</v>
+      </c>
+      <c r="AB1" t="str">
+        <v>19-Nov-</v>
+      </c>
+      <c r="AC1" t="str">
+        <v>20-Nov-</v>
+      </c>
+      <c r="AD1" t="str">
+        <v>21-Nov-</v>
+      </c>
+      <c r="AE1" t="str">
+        <v>22-Nov-</v>
+      </c>
+      <c r="AF1" t="str">
+        <v>23-Nov-</v>
+      </c>
+      <c r="AG1" t="str">
+        <v>24-Nov-</v>
+      </c>
+      <c r="AH1" t="str">
+        <v>25-Nov-</v>
+      </c>
+      <c r="AI1" t="str">
+        <v>26-Nov-</v>
+      </c>
+      <c r="AJ1" t="str">
+        <v>27-Nov-</v>
+      </c>
+      <c r="AK1" t="str">
+        <v>28-Nov-</v>
+      </c>
+      <c r="AL1" t="str">
+        <v>29-Nov-</v>
+      </c>
+      <c r="AM1" t="str">
         <v>30-Nov-</v>
       </c>
-      <c r="D1" t="str">
+      <c r="AN1" t="str">
         <v>1-Dec-</v>
       </c>
-      <c r="E1" t="str">
+      <c r="AO1" t="str">
         <v>2-Dec-</v>
       </c>
-      <c r="F1" t="str">
+      <c r="AP1" t="str">
         <v>3-Dec-</v>
       </c>
-      <c r="G1" t="str">
+      <c r="AQ1" t="str">
         <v>4-Dec-</v>
       </c>
-      <c r="H1" t="str">
+      <c r="AR1" t="str">
         <v>5-Dec-</v>
       </c>
-      <c r="I1" t="str">
+      <c r="AS1" t="str">
         <v>6-Dec-</v>
       </c>
-      <c r="J1" t="str">
+      <c r="AT1" t="str">
         <v>7-Dec-</v>
       </c>
-      <c r="K1" t="str">
+      <c r="AU1" t="str">
         <v>8-Dec-</v>
       </c>
-      <c r="L1" t="str">
+      <c r="AV1" t="str">
         <v>9-Dec-</v>
       </c>
-      <c r="M1" t="str">
+      <c r="AW1" t="str">
         <v>10-Dec-</v>
       </c>
-      <c r="N1" t="str">
+      <c r="AX1" t="str">
         <v>11-Dec-</v>
       </c>
-      <c r="O1" t="str">
+      <c r="AY1" t="str">
         <v>12-Dec-</v>
       </c>
-      <c r="P1" t="str">
+      <c r="AZ1" t="str">
         <v>13-Dec-</v>
       </c>
-      <c r="Q1" t="str">
+      <c r="BA1" t="str">
         <v>14-Dec-</v>
       </c>
-      <c r="R1" t="str">
+      <c r="BB1" t="str">
         <v>15-Dec-</v>
       </c>
-      <c r="S1" t="str">
+      <c r="BC1" t="str">
         <v>16-Dec-</v>
       </c>
-      <c r="T1" t="str">
+      <c r="BD1" t="str">
         <v>17-Dec-</v>
       </c>
-      <c r="U1" t="str">
+      <c r="BE1" t="str">
         <v>18-Dec-</v>
       </c>
-      <c r="V1" t="str">
+      <c r="BF1" t="str">
         <v>19-Dec-</v>
       </c>
-      <c r="W1" t="str">
+      <c r="BG1" t="str">
         <v>20-Dec-</v>
       </c>
-      <c r="X1" t="str">
+      <c r="BH1" t="str">
         <v>21-Dec-</v>
       </c>
-      <c r="Y1" t="str">
+      <c r="BI1" t="str">
         <v>22-Dec-</v>
       </c>
-      <c r="Z1" t="str">
+      <c r="BJ1" t="str">
         <v>23-Dec-</v>
       </c>
-      <c r="AA1" t="str">
+      <c r="BK1" t="str">
         <v>24-Dec-</v>
       </c>
-      <c r="AB1" t="str">
+      <c r="BL1" t="str">
         <v>25-Dec-</v>
       </c>
-      <c r="AC1" t="str">
+      <c r="BM1" t="str">
         <v>26-Dec-</v>
       </c>
-      <c r="AD1" t="str">
+      <c r="BN1" t="str">
         <v>27-Dec-</v>
       </c>
-      <c r="AE1" t="str">
+      <c r="BO1" t="str">
         <v>28-Dec-</v>
       </c>
-      <c r="AF1" t="str">
+      <c r="BP1" t="str">
         <v>29-Dec-</v>
       </c>
-      <c r="AG1" t="str">
+      <c r="BQ1" t="str">
         <v>30-Dec-</v>
       </c>
-      <c r="AH1" t="str">
+      <c r="BR1" t="str">
+        <v>31-Dec-</v>
+      </c>
+      <c r="BS1" t="str">
+        <v>1-Jan-</v>
+      </c>
+      <c r="BT1" t="str">
+        <v>2-Jan-</v>
+      </c>
+      <c r="BU1" t="str">
+        <v>3-Jan-</v>
+      </c>
+      <c r="BV1" t="str">
+        <v>4-Jan-</v>
+      </c>
+      <c r="BW1" t="str">
+        <v>5-Jan-</v>
+      </c>
+      <c r="BX1" t="str">
+        <v>6-Jan-</v>
+      </c>
+      <c r="BY1" t="str">
+        <v>7-Jan-</v>
+      </c>
+      <c r="BZ1" t="str">
+        <v>8-Jan-</v>
+      </c>
+      <c r="CA1" t="str">
+        <v>9-Jan-</v>
+      </c>
+      <c r="CB1" t="str">
+        <v>10-Jan-</v>
+      </c>
+      <c r="CC1" t="str">
+        <v>11-Jan-</v>
+      </c>
+      <c r="CD1" t="str">
+        <v>12-Jan-</v>
+      </c>
+      <c r="CE1" t="str">
+        <v>13-Jan-</v>
+      </c>
+      <c r="CF1" t="str">
+        <v>14-Jan-</v>
+      </c>
+      <c r="CG1" t="str">
+        <v>15-Jan-</v>
+      </c>
+      <c r="CH1" t="str">
+        <v>16-Jan-</v>
+      </c>
+      <c r="CI1" t="str">
+        <v>17-Jan-</v>
+      </c>
+      <c r="CJ1" t="str">
+        <v>18-Jan-</v>
+      </c>
+      <c r="CK1" t="str">
+        <v>19-Jan-</v>
+      </c>
+      <c r="CL1" t="str">
         <v>Grand Total</v>
       </c>
     </row>
@@ -564,13 +776,19 @@
       <c r="B2" t="str">
         <v>Evelyn Magbanua</v>
       </c>
+      <c r="CL2">
+        <v>9</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>00002</v>
+        <v>00003</v>
       </c>
       <c r="B3" t="str">
         <v>Gemry Delle Taparan</v>
+      </c>
+      <c r="CL3">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -578,15 +796,21 @@
         <v>00003</v>
       </c>
       <c r="B4" t="str">
-        <v>Jay Yhansey A. Del Rosario</v>
+        <v>Gemry Delle Taparan</v>
+      </c>
+      <c r="CL4">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>00004</v>
+        <v>00005</v>
       </c>
       <c r="B5" t="str">
-        <v>Nikki Sixx Acosta</v>
+        <v>Jay Yhansey A. Del Rosario</v>
+      </c>
+      <c r="CL5">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -594,15 +818,21 @@
         <v>00005</v>
       </c>
       <c r="B6" t="str">
-        <v>Nikki Sixx Acosta</v>
+        <v>Jay Yhansey A. Del Rosario</v>
+      </c>
+      <c r="CL6">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>00010</v>
+        <v>00006</v>
       </c>
       <c r="B7" t="str">
-        <v>please work</v>
+        <v>Nikki Sixx Acosta</v>
+      </c>
+      <c r="CL7">
+        <v>8</v>
       </c>
     </row>
     <row r="8">
@@ -612,10 +842,13 @@
       <c r="B8" t="str">
         <v>Grand Total</v>
       </c>
+      <c r="CL8">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AH8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:CL8"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -627,8 +860,8 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="15.00390625" customWidth="1"/>
-    <col min="2" max="2" width="66.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.00390625" customWidth="1"/>
+    <col min="2" max="2" width="50.00390625" customWidth="1"/>
     <col min="3" max="3" width="19.50390625" customWidth="1"/>
     <col min="4" max="4" width="32.33203125" customWidth="1"/>
     <col min="5" max="5" width="14.83203125" customWidth="1"/>
@@ -666,10 +899,16 @@
       <c r="B2" t="str">
         <v>Evelyn Magbanua</v>
       </c>
+      <c r="C2">
+        <v>70</v>
+      </c>
+      <c r="G2">
+        <v>70</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>00002</v>
+        <v>00003</v>
       </c>
       <c r="B3" t="str">
         <v>Gemry Delle Taparan</v>
@@ -680,15 +919,15 @@
         <v>00003</v>
       </c>
       <c r="B4" t="str">
-        <v>Jay Yhansey A. Del Rosario</v>
+        <v>Gemry Delle Taparan</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>00004</v>
+        <v>00005</v>
       </c>
       <c r="B5" t="str">
-        <v>Nikki Sixx Acosta</v>
+        <v>Jay Yhansey A. Del Rosario</v>
       </c>
     </row>
     <row r="6">
@@ -696,15 +935,21 @@
         <v>00005</v>
       </c>
       <c r="B6" t="str">
-        <v>Nikki Sixx Acosta</v>
+        <v>Jay Yhansey A. Del Rosario</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>00010</v>
+        <v>00006</v>
       </c>
       <c r="B7" t="str">
-        <v>please work</v>
+        <v>Nikki Sixx Acosta</v>
+      </c>
+      <c r="C7">
+        <v>99</v>
+      </c>
+      <c r="G7">
+        <v>99</v>
       </c>
     </row>
     <row r="8">
@@ -713,6 +958,12 @@
       </c>
       <c r="B8" t="str">
         <v>Grand Total</v>
+      </c>
+      <c r="C8">
+        <v>169</v>
+      </c>
+      <c r="G8">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -729,8 +980,8 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="15.00390625" customWidth="1"/>
-    <col min="2" max="2" width="66.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.00390625" customWidth="1"/>
+    <col min="2" max="2" width="50.00390625" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" customWidth="1"/>
     <col min="4" max="4" width="12.50390625" customWidth="1"/>
   </cols>
@@ -762,7 +1013,7 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>00002</v>
+        <v>00003</v>
       </c>
       <c r="B3" t="str">
         <v>Gemry Delle Taparan</v>
@@ -776,7 +1027,7 @@
         <v>00003</v>
       </c>
       <c r="B4" t="str">
-        <v>Jay Yhansey A. Del Rosario</v>
+        <v>Gemry Delle Taparan</v>
       </c>
       <c r="C4" t="str">
         <v>Tuburan</v>
@@ -784,13 +1035,13 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>00004</v>
+        <v>00005</v>
       </c>
       <c r="B5" t="str">
-        <v>Nikki Sixx Acosta</v>
+        <v>Jay Yhansey A. Del Rosario</v>
       </c>
       <c r="C5" t="str">
-        <v>Cebu</v>
+        <v>Tuburan</v>
       </c>
     </row>
     <row r="6">
@@ -798,7 +1049,7 @@
         <v>00005</v>
       </c>
       <c r="B6" t="str">
-        <v>Nikki Sixx Acosta</v>
+        <v>Jay Yhansey A. Del Rosario</v>
       </c>
       <c r="C6" t="str">
         <v>Tuburan</v>
@@ -806,13 +1057,13 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>00010</v>
+        <v>00006</v>
       </c>
       <c r="B7" t="str">
-        <v>please work</v>
+        <v>Nikki Sixx Acosta</v>
       </c>
       <c r="C7" t="str">
-        <v>Cebu</v>
+        <v>Tuburan</v>
       </c>
     </row>
     <row r="8">
@@ -841,7 +1092,7 @@
   </sheetViews>
   <cols>
     <col min="1" max="1" width="16.00390625" customWidth="1"/>
-    <col min="2" max="2" width="66.6640625" customWidth="1"/>
+    <col min="2" max="2" width="50.00390625" customWidth="1"/>
     <col min="3" max="3" width="34.6640625" customWidth="1"/>
     <col min="4" max="4" width="56.83203125" customWidth="1"/>
     <col min="5" max="5" width="48.6640625" customWidth="1"/>
@@ -882,7 +1133,7 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>00002</v>
+        <v>00003</v>
       </c>
       <c r="B3" t="str">
         <v>Gemry Delle Taparan</v>
@@ -893,15 +1144,15 @@
         <v>00003</v>
       </c>
       <c r="B4" t="str">
-        <v>Jay Yhansey A. Del Rosario</v>
+        <v>Gemry Delle Taparan</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>00004</v>
+        <v>00005</v>
       </c>
       <c r="B5" t="str">
-        <v>Nikki Sixx Acosta</v>
+        <v>Jay Yhansey A. Del Rosario</v>
       </c>
     </row>
     <row r="6">
@@ -909,15 +1160,15 @@
         <v>00005</v>
       </c>
       <c r="B6" t="str">
-        <v>Nikki Sixx Acosta</v>
+        <v>Jay Yhansey A. Del Rosario</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>00010</v>
+        <v>00006</v>
       </c>
       <c r="B7" t="str">
-        <v>please work</v>
+        <v>Nikki Sixx Acosta</v>
       </c>
     </row>
     <row r="8">

</xml_diff>